<commit_message>
fixed typo in thousand cubic meters per day
</commit_message>
<xml_diff>
--- a/utils/config/ReferenceLists/Units.xlsx
+++ b/utils/config/ReferenceLists/Units.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/sahil_bhandari_gov_bc_ca/Documents/teamdocs/GitHub/aqs-api/utils/config/ReferenceLists/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/jeremy_krogh_gov_bc_ca/Documents/Projects/2025/github_projects/aqs-api/utils/config/ReferenceLists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="204" documentId="8_{7DEAA6C1-0DF4-4EB3-B17D-DC8C9B3E57AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DE618F6-B41A-4FDB-BE1C-E4E0B3C79435}"/>
+  <xr:revisionPtr revIDLastSave="222" documentId="8_{7DEAA6C1-0DF4-4EB3-B17D-DC8C9B3E57AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5B76C80-50D0-40FD-B65F-7D418E51B3DA}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{BEB82E07-AA54-4E71-A23C-79CC3F3C1001}"/>
+    <workbookView xWindow="-10000" yWindow="-21710" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{BEB82E07-AA54-4E71-A23C-79CC3F3C1001}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1608,9 +1608,6 @@
     <t>µg/mL</t>
   </si>
   <si>
-    <t>tft³/d</t>
-  </si>
-  <si>
     <t>(count)</t>
   </si>
   <si>
@@ -1657,6 +1654,9 @@
   </si>
   <si>
     <t>OFFSET</t>
+  </si>
+  <si>
+    <t>tm³/d</t>
   </si>
 </sst>
 </file>
@@ -1724,7 +1724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1733,8 +1733,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -2076,20 +2074,20 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.54296875" customWidth="1"/>
-    <col min="3" max="3" width="50.26953125" customWidth="1"/>
-    <col min="4" max="6" width="18.54296875" customWidth="1"/>
-    <col min="7" max="7" width="23.453125" customWidth="1"/>
-    <col min="8" max="8" width="18.54296875" customWidth="1"/>
-    <col min="9" max="9" width="27.54296875" customWidth="1"/>
-    <col min="10" max="10" width="27.7265625" customWidth="1"/>
+    <col min="1" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="50.28515625" customWidth="1"/>
+    <col min="4" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="27.5703125" customWidth="1"/>
+    <col min="10" max="10" width="27.7109375" customWidth="1"/>
     <col min="11" max="12" width="27" customWidth="1"/>
-    <col min="13" max="13" width="33.1796875" customWidth="1"/>
+    <col min="13" max="13" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2130,7 +2128,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2173,7 +2171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2216,7 +2214,7 @@
         <v xml:space="preserve"> (transmittance)</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2259,7 +2257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2302,7 +2300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2345,7 +2343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -2388,7 +2386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -2431,7 +2429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -2474,7 +2472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -2517,7 +2515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -2560,7 +2558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -2603,7 +2601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -2647,7 +2645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2691,7 +2689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -2735,7 +2733,7 @@
         <v xml:space="preserve"> (by vol.)</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -2779,7 +2777,7 @@
         <v xml:space="preserve"> (wet)</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -2823,7 +2821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -2867,7 +2865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -2911,7 +2909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -2955,7 +2953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -2999,7 +2997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -3043,7 +3041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>71</v>
       </c>
@@ -3087,7 +3085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -3131,7 +3129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -3175,7 +3173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>80</v>
       </c>
@@ -3219,7 +3217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>83</v>
       </c>
@@ -3263,7 +3261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>86</v>
       </c>
@@ -3307,7 +3305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>89</v>
       </c>
@@ -3351,7 +3349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>92</v>
       </c>
@@ -3395,7 +3393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>95</v>
       </c>
@@ -3439,7 +3437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>98</v>
       </c>
@@ -3483,7 +3481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>101</v>
       </c>
@@ -3527,7 +3525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -3571,7 +3569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>107</v>
       </c>
@@ -3615,7 +3613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>110</v>
       </c>
@@ -3659,7 +3657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>113</v>
       </c>
@@ -3703,7 +3701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -3747,7 +3745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>118</v>
       </c>
@@ -3791,7 +3789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>121</v>
       </c>
@@ -3835,7 +3833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>124</v>
       </c>
@@ -3879,7 +3877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>127</v>
       </c>
@@ -3923,7 +3921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>130</v>
       </c>
@@ -3967,7 +3965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>133</v>
       </c>
@@ -4011,7 +4009,7 @@
         <v xml:space="preserve"> (wet)</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>136</v>
       </c>
@@ -4055,7 +4053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>139</v>
       </c>
@@ -4099,7 +4097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>142</v>
       </c>
@@ -4143,7 +4141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>145</v>
       </c>
@@ -4187,7 +4185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>148</v>
       </c>
@@ -4231,7 +4229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>151</v>
       </c>
@@ -4275,7 +4273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>154</v>
       </c>
@@ -4319,7 +4317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>157</v>
       </c>
@@ -4363,7 +4361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>160</v>
       </c>
@@ -4407,7 +4405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>163</v>
       </c>
@@ -4451,7 +4449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>166</v>
       </c>
@@ -4495,7 +4493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>169</v>
       </c>
@@ -4539,7 +4537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>172</v>
       </c>
@@ -4583,7 +4581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>175</v>
       </c>
@@ -4627,7 +4625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>178</v>
       </c>
@@ -4671,7 +4669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>181</v>
       </c>
@@ -4715,7 +4713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>184</v>
       </c>
@@ -4759,7 +4757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>187</v>
       </c>
@@ -4803,7 +4801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>190</v>
       </c>
@@ -4847,7 +4845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>193</v>
       </c>
@@ -4891,7 +4889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>196</v>
       </c>
@@ -4935,7 +4933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>199</v>
       </c>
@@ -4979,7 +4977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>202</v>
       </c>
@@ -5023,7 +5021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>205</v>
       </c>
@@ -5067,7 +5065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>208</v>
       </c>
@@ -5111,7 +5109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>211</v>
       </c>
@@ -5155,7 +5153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>214</v>
       </c>
@@ -5199,7 +5197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>217</v>
       </c>
@@ -5243,7 +5241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>220</v>
       </c>
@@ -5287,7 +5285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>223</v>
       </c>
@@ -5331,7 +5329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>226</v>
       </c>
@@ -5375,7 +5373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>229</v>
       </c>
@@ -5419,7 +5417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>232</v>
       </c>
@@ -5463,7 +5461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>235</v>
       </c>
@@ -5507,7 +5505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>238</v>
       </c>
@@ -5551,7 +5549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>241</v>
       </c>
@@ -5595,7 +5593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>244</v>
       </c>
@@ -5639,7 +5637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>247</v>
       </c>
@@ -5683,7 +5681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>250</v>
       </c>
@@ -5727,7 +5725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>253</v>
       </c>
@@ -5771,7 +5769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>256</v>
       </c>
@@ -5815,7 +5813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>259</v>
       </c>
@@ -5859,7 +5857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>262</v>
       </c>
@@ -5903,7 +5901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>265</v>
       </c>
@@ -5947,7 +5945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>268</v>
       </c>
@@ -5991,7 +5989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>271</v>
       </c>
@@ -6035,7 +6033,7 @@
         <v xml:space="preserve"> (mortality)</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>274</v>
       </c>
@@ -6079,7 +6077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>277</v>
       </c>
@@ -6123,7 +6121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>280</v>
       </c>
@@ -6167,7 +6165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>283</v>
       </c>
@@ -6211,7 +6209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>286</v>
       </c>
@@ -6255,7 +6253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>289</v>
       </c>
@@ -6299,7 +6297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>291</v>
       </c>
@@ -6343,7 +6341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>294</v>
       </c>
@@ -6387,7 +6385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>296</v>
       </c>
@@ -6431,7 +6429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>299</v>
       </c>
@@ -6475,7 +6473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>302</v>
       </c>
@@ -6519,7 +6517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>305</v>
       </c>
@@ -6563,7 +6561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>308</v>
       </c>
@@ -6607,7 +6605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>311</v>
       </c>
@@ -6651,7 +6649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>314</v>
       </c>
@@ -6695,7 +6693,7 @@
         <v xml:space="preserve"> (wet)</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>317</v>
       </c>
@@ -6739,7 +6737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>319</v>
       </c>
@@ -6783,7 +6781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>322</v>
       </c>
@@ -6827,7 +6825,7 @@
         <v xml:space="preserve"> (LEL)</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>325</v>
       </c>
@@ -6871,7 +6869,7 @@
         <v xml:space="preserve"> (saturation)</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>327</v>
       </c>
@@ -6915,7 +6913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>330</v>
       </c>
@@ -6959,7 +6957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>333</v>
       </c>
@@ -7003,7 +7001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>336</v>
       </c>
@@ -7047,7 +7045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>339</v>
       </c>
@@ -7091,7 +7089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>342</v>
       </c>
@@ -7135,7 +7133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>345</v>
       </c>
@@ -7179,7 +7177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>348</v>
       </c>
@@ -7238,17 +7236,17 @@
       <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" customWidth="1"/>
-    <col min="2" max="2" width="32.7265625" customWidth="1"/>
-    <col min="3" max="6" width="22.26953125" customWidth="1"/>
-    <col min="7" max="7" width="27.26953125" customWidth="1"/>
-    <col min="8" max="8" width="39.26953125" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="3" max="6" width="22.28515625" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" customWidth="1"/>
+    <col min="8" max="8" width="39.28515625" customWidth="1"/>
     <col min="9" max="9" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>352</v>
       </c>
@@ -7277,7 +7275,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -7294,7 +7292,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -7311,7 +7309,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -7328,7 +7326,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -7345,7 +7343,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -7365,7 +7363,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -7382,7 +7380,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>254</v>
       </c>
@@ -7399,7 +7397,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>102</v>
       </c>
@@ -7416,7 +7414,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -7433,7 +7431,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>108</v>
       </c>
@@ -7450,7 +7448,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -7467,7 +7465,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -7484,7 +7482,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>96</v>
       </c>
@@ -7501,7 +7499,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>116</v>
       </c>
@@ -7518,7 +7516,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -7535,7 +7533,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -7552,7 +7550,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -7572,7 +7570,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -7589,7 +7587,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -7606,7 +7604,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>90</v>
       </c>
@@ -7623,7 +7621,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>111</v>
       </c>
@@ -7640,7 +7638,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>105</v>
       </c>
@@ -7657,7 +7655,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>134</v>
       </c>
@@ -7677,7 +7675,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -7694,7 +7692,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -7711,7 +7709,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -7728,7 +7726,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -7745,7 +7743,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>343</v>
       </c>
@@ -7762,7 +7760,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>78</v>
       </c>
@@ -7779,7 +7777,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>81</v>
       </c>
@@ -7796,7 +7794,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>248</v>
       </c>
@@ -7813,7 +7811,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>263</v>
       </c>
@@ -7830,7 +7828,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -7847,7 +7845,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>260</v>
       </c>
@@ -7864,7 +7862,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>272</v>
       </c>
@@ -7884,7 +7882,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>99</v>
       </c>
@@ -7901,7 +7899,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>257</v>
       </c>
@@ -7918,7 +7916,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -7935,7 +7933,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>306</v>
       </c>
@@ -7952,7 +7950,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -7969,7 +7967,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>318</v>
       </c>
@@ -7986,7 +7984,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>60</v>
       </c>
@@ -8003,7 +8001,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>340</v>
       </c>
@@ -8020,7 +8018,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>443</v>
       </c>
@@ -8037,7 +8035,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>334</v>
       </c>
@@ -8054,7 +8052,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>137</v>
       </c>
@@ -8071,7 +8069,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>122</v>
       </c>
@@ -8088,7 +8086,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>448</v>
       </c>
@@ -8105,7 +8103,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>452</v>
       </c>
@@ -8122,7 +8120,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>320</v>
       </c>
@@ -8139,7 +8137,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>143</v>
       </c>
@@ -8156,7 +8154,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>146</v>
       </c>
@@ -8173,7 +8171,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>323</v>
       </c>
@@ -8193,7 +8191,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>152</v>
       </c>
@@ -8210,7 +8208,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>457</v>
       </c>
@@ -8227,7 +8225,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>326</v>
       </c>
@@ -8247,7 +8245,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>462</v>
       </c>
@@ -8264,7 +8262,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>66</v>
       </c>
@@ -8281,7 +8279,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>465</v>
       </c>
@@ -8298,7 +8296,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>158</v>
       </c>
@@ -8315,7 +8313,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>275</v>
       </c>
@@ -8332,7 +8330,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>349</v>
       </c>
@@ -8349,7 +8347,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>468</v>
       </c>
@@ -8366,7 +8364,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>328</v>
       </c>
@@ -8383,7 +8381,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>13</v>
       </c>
@@ -8403,7 +8401,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>337</v>
       </c>
@@ -8420,7 +8418,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>93</v>
       </c>
@@ -8437,7 +8435,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>472</v>
       </c>
@@ -8454,7 +8452,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>128</v>
       </c>
@@ -8471,7 +8469,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>475</v>
       </c>
@@ -8488,7 +8486,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>119</v>
       </c>
@@ -8505,7 +8503,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>476</v>
       </c>
@@ -8522,7 +8520,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>477</v>
       </c>
@@ -8539,7 +8537,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>478</v>
       </c>
@@ -8556,7 +8554,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>479</v>
       </c>
@@ -8573,7 +8571,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>315</v>
       </c>
@@ -8593,7 +8591,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>155</v>
       </c>
@@ -8618,35 +8616,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3036B1CA-FBEB-4E41-A2A1-61CD7E3CC4C8}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="A109" sqref="A109"/>
-      <selection pane="topRight" activeCell="H83" sqref="H83"/>
+      <selection pane="topRight" activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="25.81640625" customWidth="1"/>
-    <col min="3" max="3" width="42.81640625" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="42.85546875" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="17.7265625" customWidth="1"/>
-    <col min="6" max="7" width="16.7265625" customWidth="1"/>
-    <col min="8" max="8" width="20.7265625" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" customWidth="1"/>
-    <col min="10" max="10" width="8.7265625" customWidth="1"/>
-    <col min="11" max="11" width="20.54296875" customWidth="1"/>
-    <col min="12" max="12" width="33.54296875" customWidth="1"/>
-    <col min="13" max="13" width="29.26953125" customWidth="1"/>
-    <col min="14" max="14" width="40.1796875" customWidth="1"/>
-    <col min="15" max="15" width="23.1796875" customWidth="1"/>
-    <col min="16" max="16" width="19.81640625" customWidth="1"/>
-    <col min="17" max="17" width="15.54296875" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+    <col min="12" max="12" width="33.5703125" customWidth="1"/>
+    <col min="13" max="13" width="29.28515625" customWidth="1"/>
+    <col min="14" max="14" width="40.140625" customWidth="1"/>
+    <col min="15" max="15" width="23.140625" customWidth="1"/>
+    <col min="16" max="16" width="19.85546875" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -8666,25 +8665,25 @@
         <v>351</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>353</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>355</v>
@@ -8697,7 +8696,7 @@
       </c>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>113</v>
       </c>
@@ -8744,7 +8743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>271</v>
       </c>
@@ -8791,7 +8790,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>311</v>
       </c>
@@ -8832,13 +8831,13 @@
         <v>115</v>
       </c>
       <c r="O4" t="s">
+        <v>519</v>
+      </c>
+      <c r="P4" t="s">
         <v>520</v>
       </c>
-      <c r="P4" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>322</v>
       </c>
@@ -8885,7 +8884,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>325</v>
       </c>
@@ -8932,7 +8931,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -8979,7 +8978,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>47</v>
       </c>
@@ -9026,7 +9025,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>50</v>
       </c>
@@ -9073,7 +9072,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>336</v>
       </c>
@@ -9120,7 +9119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>256</v>
       </c>
@@ -9167,7 +9166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>327</v>
       </c>
@@ -9214,7 +9213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>62</v>
       </c>
@@ -9261,7 +9260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>107</v>
       </c>
@@ -9311,7 +9310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>296</v>
       </c>
@@ -9346,19 +9345,19 @@
         <v>318</v>
       </c>
       <c r="M15" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="N15" t="s">
         <v>298</v>
       </c>
       <c r="O15" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="P15" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>299</v>
       </c>
@@ -9399,13 +9398,13 @@
         <v>301</v>
       </c>
       <c r="O16" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="P16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>193</v>
       </c>
@@ -9456,7 +9455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>77</v>
       </c>
@@ -9503,7 +9502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>319</v>
       </c>
@@ -9550,7 +9549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>32</v>
       </c>
@@ -9594,7 +9593,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>317</v>
       </c>
@@ -9641,7 +9640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>348</v>
       </c>
@@ -9692,7 +9691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>280</v>
       </c>
@@ -9730,7 +9729,7 @@
         <v>389</v>
       </c>
       <c r="M23" t="s">
-        <v>515</v>
+        <v>531</v>
       </c>
       <c r="N23" t="s">
         <v>282</v>
@@ -9742,57 +9741,57 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="8" t="s">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" t="s">
         <v>173</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" t="s">
         <v>174</v>
       </c>
-      <c r="D24" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="9" t="s">
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="F24" t="s">
         <v>116</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G24" t="s">
         <v>116</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24">
         <v>4546.09</v>
       </c>
-      <c r="I24" s="9">
-        <v>0</v>
-      </c>
-      <c r="J24" s="9">
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
         <v>176</v>
       </c>
-      <c r="K24" s="9" t="b">
+      <c r="K24" t="b">
         <v>1</v>
       </c>
-      <c r="L24" s="9" t="s">
+      <c r="L24" t="s">
         <v>389</v>
       </c>
-      <c r="M24" s="9" t="s">
+      <c r="M24" t="s">
         <v>500</v>
       </c>
-      <c r="N24" s="9" t="s">
+      <c r="N24" t="s">
         <v>174</v>
       </c>
-      <c r="O24" s="9" t="s">
+      <c r="O24" t="s">
         <v>391</v>
       </c>
-      <c r="P24" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>178</v>
       </c>
@@ -9842,7 +9841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>232</v>
       </c>
@@ -9893,7 +9892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>65</v>
       </c>
@@ -9931,7 +9930,7 @@
         <v>490</v>
       </c>
       <c r="N27" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="O27" t="s">
         <v>460</v>
@@ -9940,7 +9939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>166</v>
       </c>
@@ -9991,7 +9990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>139</v>
       </c>
@@ -10041,7 +10040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>53</v>
       </c>
@@ -10091,7 +10090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>259</v>
       </c>
@@ -10141,7 +10140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>169</v>
       </c>
@@ -10192,7 +10191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>244</v>
       </c>
@@ -10236,7 +10235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>253</v>
       </c>
@@ -10283,7 +10282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>214</v>
       </c>
@@ -10330,7 +10329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>229</v>
       </c>
@@ -10381,58 +10380,58 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="8" t="s">
+    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" t="s">
         <v>149</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" t="s">
         <v>150</v>
       </c>
-      <c r="D37" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="9" t="s">
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" t="s">
         <v>18</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="F37" t="s">
         <v>19</v>
       </c>
-      <c r="G37" s="9" t="s">
+      <c r="G37" t="s">
         <v>57</v>
       </c>
-      <c r="H37" s="9">
+      <c r="H37">
         <f>1000000000</f>
         <v>1000000000</v>
       </c>
-      <c r="I37" s="9">
-        <v>0</v>
-      </c>
-      <c r="J37" s="9">
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
         <v>16</v>
       </c>
-      <c r="K37" s="9" t="b">
+      <c r="K37" t="b">
         <v>1</v>
       </c>
-      <c r="L37" s="9" t="s">
+      <c r="L37" t="s">
         <v>407</v>
       </c>
-      <c r="M37" s="9" t="s">
+      <c r="M37" t="s">
         <v>497</v>
       </c>
-      <c r="N37" s="9" t="s">
+      <c r="N37" t="s">
         <v>150</v>
       </c>
-      <c r="O37" s="9" t="s">
+      <c r="O37" t="s">
         <v>409</v>
       </c>
-      <c r="P37" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="P37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>286</v>
       </c>
@@ -10482,7 +10481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>95</v>
       </c>
@@ -10532,7 +10531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>71</v>
       </c>
@@ -10583,7 +10582,7 @@
       </c>
       <c r="Q40"/>
     </row>
-    <row r="41" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>175</v>
       </c>
@@ -10635,7 +10634,7 @@
       </c>
       <c r="Q41"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>250</v>
       </c>
@@ -10686,7 +10685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>283</v>
       </c>
@@ -10737,7 +10736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>83</v>
       </c>
@@ -10787,7 +10786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>104</v>
       </c>
@@ -10837,7 +10836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>157</v>
       </c>
@@ -10887,7 +10886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>11</v>
       </c>
@@ -10937,7 +10936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>187</v>
       </c>
@@ -10987,58 +10986,58 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="8" t="s">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" t="s">
         <v>236</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C49" t="s">
         <v>237</v>
       </c>
-      <c r="D49" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E49" s="9" t="s">
+      <c r="D49" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" t="s">
         <v>11</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="F49" t="s">
         <v>116</v>
       </c>
-      <c r="G49" s="9" t="s">
+      <c r="G49" t="s">
         <v>116</v>
       </c>
-      <c r="H49" s="9">
+      <c r="H49">
         <f>1/30</f>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="I49" s="9">
-        <v>0</v>
-      </c>
-      <c r="J49" s="9">
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
         <v>6</v>
       </c>
-      <c r="K49" s="9" t="b">
+      <c r="K49" t="b">
         <v>1</v>
       </c>
-      <c r="L49" s="9" t="s">
+      <c r="L49" t="s">
         <v>389</v>
       </c>
-      <c r="M49" s="9" t="s">
+      <c r="M49" t="s">
         <v>511</v>
       </c>
-      <c r="N49" s="9" t="s">
+      <c r="N49" t="s">
         <v>237</v>
       </c>
-      <c r="O49" s="9" t="s">
+      <c r="O49" t="s">
         <v>391</v>
       </c>
-      <c r="P49" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>184</v>
       </c>
@@ -11089,7 +11088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>92</v>
       </c>
@@ -11140,7 +11139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>7</v>
       </c>
@@ -11188,7 +11187,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="53" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>190</v>
       </c>
@@ -11240,7 +11239,7 @@
       </c>
       <c r="Q53"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>89</v>
       </c>
@@ -11291,7 +11290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>238</v>
       </c>
@@ -11342,58 +11341,58 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="8" t="s">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="B56" t="s">
         <v>242</v>
       </c>
-      <c r="C56" s="9" t="s">
+      <c r="C56" t="s">
         <v>243</v>
       </c>
-      <c r="D56" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E56" s="9" t="s">
+      <c r="D56" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="9" t="s">
+      <c r="F56" t="s">
         <v>116</v>
       </c>
-      <c r="G56" s="9" t="s">
+      <c r="G56" t="s">
         <v>116</v>
       </c>
-      <c r="H56" s="9">
+      <c r="H56">
         <f>1/365.25</f>
         <v>2.7378507871321013E-3</v>
       </c>
-      <c r="I56" s="9">
-        <v>0</v>
-      </c>
-      <c r="J56" s="9">
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
         <v>12</v>
       </c>
-      <c r="K56" s="9" t="b">
+      <c r="K56" t="b">
         <v>1</v>
       </c>
-      <c r="L56" s="9" t="s">
+      <c r="L56" t="s">
         <v>389</v>
       </c>
-      <c r="M56" s="9" t="s">
+      <c r="M56" t="s">
         <v>513</v>
       </c>
-      <c r="N56" s="9" t="s">
+      <c r="N56" t="s">
         <v>243</v>
       </c>
-      <c r="O56" s="9" t="s">
+      <c r="O56" t="s">
         <v>391</v>
       </c>
-      <c r="P56" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>333</v>
       </c>
@@ -11413,7 +11412,7 @@
         <v>0</v>
       </c>
       <c r="G57" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H57">
         <v>1000</v>
@@ -11431,7 +11430,7 @@
         <v>433</v>
       </c>
       <c r="M57" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="N57" t="s">
         <v>335</v>
@@ -11444,7 +11443,7 @@
       </c>
       <c r="Q57"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>24</v>
       </c>
@@ -11491,7 +11490,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>59</v>
       </c>
@@ -11541,7 +11540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>205</v>
       </c>
@@ -11593,7 +11592,7 @@
       </c>
       <c r="Q60"/>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>211</v>
       </c>
@@ -11643,7 +11642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>217</v>
       </c>
@@ -11693,7 +11692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>220</v>
       </c>
@@ -11743,7 +11742,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>18</v>
       </c>
@@ -11790,7 +11789,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>223</v>
       </c>
@@ -11841,7 +11840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>124</v>
       </c>
@@ -11891,7 +11890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>160</v>
       </c>
@@ -11941,7 +11940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>44</v>
       </c>
@@ -11988,7 +11987,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>118</v>
       </c>
@@ -12039,7 +12038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>196</v>
       </c>
@@ -12090,7 +12089,7 @@
       </c>
       <c r="Q70" s="3"/>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>247</v>
       </c>
@@ -12137,7 +12136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>80</v>
       </c>
@@ -12184,7 +12183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>262</v>
       </c>
@@ -12231,7 +12230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>345</v>
       </c>
@@ -12269,7 +12268,7 @@
         <v>378</v>
       </c>
       <c r="M74" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N74" t="s">
         <v>347</v>
@@ -12281,7 +12280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>110</v>
       </c>
@@ -12328,7 +12327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>289</v>
       </c>
@@ -12379,7 +12378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>142</v>
       </c>
@@ -12430,7 +12429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>291</v>
       </c>
@@ -12471,13 +12470,13 @@
         <v>293</v>
       </c>
       <c r="O78" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="P78" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>308</v>
       </c>
@@ -12512,19 +12511,19 @@
         <v>318</v>
       </c>
       <c r="M79" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="N79" t="s">
         <v>310</v>
       </c>
       <c r="O79" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="P79" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>15</v>
       </c>
@@ -12568,7 +12567,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>35</v>
       </c>
@@ -12609,7 +12608,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>136</v>
       </c>
@@ -12661,7 +12660,7 @@
       </c>
       <c r="Q82" s="3"/>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>314</v>
       </c>
@@ -12713,7 +12712,7 @@
       </c>
       <c r="Q83" s="3"/>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>121</v>
       </c>
@@ -12764,7 +12763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>30</v>
       </c>
@@ -12808,7 +12807,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>154</v>
       </c>
@@ -12846,7 +12845,7 @@
         <v>482</v>
       </c>
       <c r="N86" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="O86" t="s">
         <v>411</v>
@@ -12855,7 +12854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>339</v>
       </c>
@@ -12893,7 +12892,7 @@
         <v>442</v>
       </c>
       <c r="N87" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="O87" t="s">
         <v>411</v>
@@ -12902,7 +12901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>151</v>
       </c>
@@ -12940,7 +12939,7 @@
         <v>442</v>
       </c>
       <c r="N88" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="O88" t="s">
         <v>411</v>
@@ -12949,7 +12948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>145</v>
       </c>
@@ -12987,7 +12986,7 @@
         <v>442</v>
       </c>
       <c r="N89" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="O89" t="s">
         <v>411</v>
@@ -12996,7 +12995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>74</v>
       </c>
@@ -13043,7 +13042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>342</v>
       </c>
@@ -13090,7 +13089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>41</v>
       </c>
@@ -13134,7 +13133,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="93" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:17" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
         <v>98</v>
       </c>
@@ -13156,7 +13155,7 @@
       <c r="G93" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H93" s="10">
+      <c r="H93" s="8">
         <f>1000000000</f>
         <v>1000000000</v>
       </c>
@@ -13185,7 +13184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>101</v>
       </c>
@@ -13235,7 +13234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>274</v>
       </c>
@@ -13285,7 +13284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>38</v>
       </c>
@@ -13329,7 +13328,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>330</v>
       </c>
@@ -13370,13 +13369,13 @@
         <v>332</v>
       </c>
       <c r="O97" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="P97" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>226</v>
       </c>
@@ -13426,7 +13425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>68</v>
       </c>
@@ -13446,7 +13445,7 @@
         <v>0</v>
       </c>
       <c r="G99" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H99">
         <v>1</v>
@@ -13476,7 +13475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>208</v>
       </c>
@@ -13527,7 +13526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>130</v>
       </c>
@@ -13578,7 +13577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>86</v>
       </c>
@@ -13628,7 +13627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>199</v>
       </c>
@@ -13679,7 +13678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>202</v>
       </c>
@@ -13730,7 +13729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>21</v>
       </c>
@@ -13777,7 +13776,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>133</v>
       </c>
@@ -13827,7 +13826,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>302</v>
       </c>
@@ -13866,7 +13865,7 @@
         <v>368</v>
       </c>
       <c r="M107" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="N107" t="s">
         <v>304</v>
@@ -13878,7 +13877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>127</v>
       </c>
@@ -13929,7 +13928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>56</v>
       </c>
@@ -13979,7 +13978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:17" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>268</v>
       </c>
@@ -14030,7 +14029,7 @@
       </c>
       <c r="Q110"/>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>163</v>
       </c>
@@ -14080,7 +14079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>305</v>
       </c>
@@ -14130,7 +14129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:17" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>27</v>
       </c>
@@ -14179,7 +14178,7 @@
       <c r="P113"/>
       <c r="Q113"/>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>277</v>
       </c>
@@ -14230,7 +14229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>181</v>
       </c>
@@ -14281,7 +14280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>294</v>
       </c>
@@ -14322,14 +14321,20 @@
         <v>295</v>
       </c>
       <c r="O116" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="P116" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q116" xr:uid="{3036B1CA-FBEB-4E41-A2A1-61CD7E3CC4C8}"/>
+  <autoFilter ref="A1:Q116" xr:uid="{3036B1CA-FBEB-4E41-A2A1-61CD7E3CC4C8}">
+    <filterColumn colId="11">
+      <filters>
+        <filter val="Flow"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q116">
     <sortCondition ref="B2:B116"/>
   </sortState>

</xml_diff>

<commit_message>
Updated unit processing to gen consolidated file
</commit_message>
<xml_diff>
--- a/utils/config/ReferenceLists/Units.xlsx
+++ b/utils/config/ReferenceLists/Units.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/jeremy_krogh_gov_bc_ca/Documents/Projects/2025/github_projects/aqs-api/utils/config/ReferenceLists/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/sahil_bhandari_gov_bc_ca/Documents/teamdocs/GitHub/aqs-api/utils/config/ReferenceLists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="222" documentId="8_{7DEAA6C1-0DF4-4EB3-B17D-DC8C9B3E57AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5B76C80-50D0-40FD-B65F-7D418E51B3DA}"/>
+  <xr:revisionPtr revIDLastSave="228" documentId="8_{7DEAA6C1-0DF4-4EB3-B17D-DC8C9B3E57AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDF16032-C2E6-4145-81D5-FD6D3A0D9769}"/>
   <bookViews>
-    <workbookView xWindow="-10000" yWindow="-21710" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{BEB82E07-AA54-4E71-A23C-79CC3F3C1001}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{BEB82E07-AA54-4E71-A23C-79CC3F3C1001}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2283" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2283" uniqueCount="531">
   <si>
     <t>CODE</t>
   </si>
@@ -1618,9 +1618,6 @@
   </si>
   <si>
     <t>No/m²</t>
-  </si>
-  <si>
-    <t>(percent)</t>
   </si>
   <si>
     <t xml:space="preserve"> (recovery)</t>
@@ -2074,20 +2071,20 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="50.28515625" customWidth="1"/>
-    <col min="4" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="9" max="9" width="27.5703125" customWidth="1"/>
-    <col min="10" max="10" width="27.7109375" customWidth="1"/>
+    <col min="1" max="2" width="18.54296875" customWidth="1"/>
+    <col min="3" max="3" width="50.26953125" customWidth="1"/>
+    <col min="4" max="6" width="18.54296875" customWidth="1"/>
+    <col min="7" max="7" width="23.453125" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" customWidth="1"/>
+    <col min="9" max="9" width="27.54296875" customWidth="1"/>
+    <col min="10" max="10" width="27.7265625" customWidth="1"/>
     <col min="11" max="12" width="27" customWidth="1"/>
-    <col min="13" max="13" width="33.140625" customWidth="1"/>
+    <col min="13" max="13" width="33.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2128,7 +2125,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2171,7 +2168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2214,7 +2211,7 @@
         <v xml:space="preserve"> (transmittance)</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2257,7 +2254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2300,7 +2297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2343,7 +2340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -2386,7 +2383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -2429,7 +2426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -2472,7 +2469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -2515,7 +2512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -2558,7 +2555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -2601,7 +2598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -2645,7 +2642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2689,7 +2686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -2733,7 +2730,7 @@
         <v xml:space="preserve"> (by vol.)</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -2777,7 +2774,7 @@
         <v xml:space="preserve"> (wet)</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -2821,7 +2818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -2865,7 +2862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -2909,7 +2906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -2953,7 +2950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -2997,7 +2994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -3041,7 +3038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>71</v>
       </c>
@@ -3085,7 +3082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -3129,7 +3126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -3173,7 +3170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>80</v>
       </c>
@@ -3217,7 +3214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>83</v>
       </c>
@@ -3261,7 +3258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>86</v>
       </c>
@@ -3305,7 +3302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>89</v>
       </c>
@@ -3349,7 +3346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>92</v>
       </c>
@@ -3393,7 +3390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>95</v>
       </c>
@@ -3437,7 +3434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>98</v>
       </c>
@@ -3481,7 +3478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>101</v>
       </c>
@@ -3525,7 +3522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -3569,7 +3566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>107</v>
       </c>
@@ -3613,7 +3610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>110</v>
       </c>
@@ -3657,7 +3654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>113</v>
       </c>
@@ -3701,7 +3698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -3745,7 +3742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>118</v>
       </c>
@@ -3789,7 +3786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>121</v>
       </c>
@@ -3833,7 +3830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>124</v>
       </c>
@@ -3877,7 +3874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>127</v>
       </c>
@@ -3921,7 +3918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>130</v>
       </c>
@@ -3965,7 +3962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>133</v>
       </c>
@@ -4009,7 +4006,7 @@
         <v xml:space="preserve"> (wet)</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>136</v>
       </c>
@@ -4053,7 +4050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>139</v>
       </c>
@@ -4097,7 +4094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>142</v>
       </c>
@@ -4141,7 +4138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>145</v>
       </c>
@@ -4185,7 +4182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>148</v>
       </c>
@@ -4229,7 +4226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>151</v>
       </c>
@@ -4273,7 +4270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>154</v>
       </c>
@@ -4317,7 +4314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>157</v>
       </c>
@@ -4361,7 +4358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>160</v>
       </c>
@@ -4405,7 +4402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>163</v>
       </c>
@@ -4449,7 +4446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>166</v>
       </c>
@@ -4493,7 +4490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>169</v>
       </c>
@@ -4537,7 +4534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>172</v>
       </c>
@@ -4581,7 +4578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>175</v>
       </c>
@@ -4625,7 +4622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>178</v>
       </c>
@@ -4669,7 +4666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>181</v>
       </c>
@@ -4713,7 +4710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>184</v>
       </c>
@@ -4757,7 +4754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>187</v>
       </c>
@@ -4801,7 +4798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>190</v>
       </c>
@@ -4845,7 +4842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>193</v>
       </c>
@@ -4889,7 +4886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>196</v>
       </c>
@@ -4933,7 +4930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>199</v>
       </c>
@@ -4977,7 +4974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>202</v>
       </c>
@@ -5021,7 +5018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>205</v>
       </c>
@@ -5065,7 +5062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>208</v>
       </c>
@@ -5109,7 +5106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>211</v>
       </c>
@@ -5153,7 +5150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>214</v>
       </c>
@@ -5197,7 +5194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>217</v>
       </c>
@@ -5241,7 +5238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>220</v>
       </c>
@@ -5285,7 +5282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>223</v>
       </c>
@@ -5329,7 +5326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>226</v>
       </c>
@@ -5373,7 +5370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>229</v>
       </c>
@@ -5417,7 +5414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>232</v>
       </c>
@@ -5461,7 +5458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>235</v>
       </c>
@@ -5505,7 +5502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>238</v>
       </c>
@@ -5549,7 +5546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>241</v>
       </c>
@@ -5593,7 +5590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>244</v>
       </c>
@@ -5637,7 +5634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>247</v>
       </c>
@@ -5681,7 +5678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>250</v>
       </c>
@@ -5725,7 +5722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>253</v>
       </c>
@@ -5769,7 +5766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>256</v>
       </c>
@@ -5813,7 +5810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>259</v>
       </c>
@@ -5857,7 +5854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>262</v>
       </c>
@@ -5901,7 +5898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>265</v>
       </c>
@@ -5945,7 +5942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>268</v>
       </c>
@@ -5989,7 +5986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>271</v>
       </c>
@@ -6033,7 +6030,7 @@
         <v xml:space="preserve"> (mortality)</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>274</v>
       </c>
@@ -6077,7 +6074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>277</v>
       </c>
@@ -6121,7 +6118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>280</v>
       </c>
@@ -6165,7 +6162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>283</v>
       </c>
@@ -6209,7 +6206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>286</v>
       </c>
@@ -6253,7 +6250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>289</v>
       </c>
@@ -6297,7 +6294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>291</v>
       </c>
@@ -6341,7 +6338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>294</v>
       </c>
@@ -6385,7 +6382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>296</v>
       </c>
@@ -6429,7 +6426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>299</v>
       </c>
@@ -6473,7 +6470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>302</v>
       </c>
@@ -6517,7 +6514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>305</v>
       </c>
@@ -6561,7 +6558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>308</v>
       </c>
@@ -6605,7 +6602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>311</v>
       </c>
@@ -6649,7 +6646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>314</v>
       </c>
@@ -6693,7 +6690,7 @@
         <v xml:space="preserve"> (wet)</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>317</v>
       </c>
@@ -6737,7 +6734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>319</v>
       </c>
@@ -6781,7 +6778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>322</v>
       </c>
@@ -6825,7 +6822,7 @@
         <v xml:space="preserve"> (LEL)</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>325</v>
       </c>
@@ -6869,7 +6866,7 @@
         <v xml:space="preserve"> (saturation)</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>327</v>
       </c>
@@ -6913,7 +6910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>330</v>
       </c>
@@ -6957,7 +6954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>333</v>
       </c>
@@ -7001,7 +6998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>336</v>
       </c>
@@ -7045,7 +7042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>339</v>
       </c>
@@ -7089,7 +7086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>342</v>
       </c>
@@ -7133,7 +7130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>345</v>
       </c>
@@ -7177,7 +7174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>348</v>
       </c>
@@ -7236,17 +7233,17 @@
       <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1"/>
-    <col min="3" max="6" width="22.28515625" customWidth="1"/>
-    <col min="7" max="7" width="27.28515625" customWidth="1"/>
-    <col min="8" max="8" width="39.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.81640625" customWidth="1"/>
+    <col min="2" max="2" width="32.7265625" customWidth="1"/>
+    <col min="3" max="6" width="22.26953125" customWidth="1"/>
+    <col min="7" max="7" width="27.26953125" customWidth="1"/>
+    <col min="8" max="8" width="39.26953125" customWidth="1"/>
     <col min="9" max="9" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>352</v>
       </c>
@@ -7275,7 +7272,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -7292,7 +7289,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -7309,7 +7306,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -7326,7 +7323,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -7343,7 +7340,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -7363,7 +7360,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -7380,7 +7377,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>254</v>
       </c>
@@ -7397,7 +7394,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>102</v>
       </c>
@@ -7414,7 +7411,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -7431,7 +7428,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>108</v>
       </c>
@@ -7448,7 +7445,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -7465,7 +7462,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -7482,7 +7479,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>96</v>
       </c>
@@ -7499,7 +7496,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>116</v>
       </c>
@@ -7516,7 +7513,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -7533,7 +7530,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -7550,7 +7547,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -7570,7 +7567,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -7587,7 +7584,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -7604,7 +7601,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>90</v>
       </c>
@@ -7621,7 +7618,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>111</v>
       </c>
@@ -7638,7 +7635,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>105</v>
       </c>
@@ -7655,7 +7652,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>134</v>
       </c>
@@ -7675,7 +7672,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -7692,7 +7689,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -7709,7 +7706,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -7726,7 +7723,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -7743,7 +7740,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>343</v>
       </c>
@@ -7760,7 +7757,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>78</v>
       </c>
@@ -7777,7 +7774,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>81</v>
       </c>
@@ -7794,7 +7791,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>248</v>
       </c>
@@ -7811,7 +7808,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>263</v>
       </c>
@@ -7828,7 +7825,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -7845,7 +7842,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>260</v>
       </c>
@@ -7862,7 +7859,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>272</v>
       </c>
@@ -7882,7 +7879,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>99</v>
       </c>
@@ -7899,7 +7896,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>257</v>
       </c>
@@ -7916,7 +7913,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -7933,7 +7930,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>306</v>
       </c>
@@ -7950,7 +7947,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -7967,7 +7964,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>318</v>
       </c>
@@ -7984,7 +7981,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>60</v>
       </c>
@@ -8001,7 +7998,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>340</v>
       </c>
@@ -8018,7 +8015,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>443</v>
       </c>
@@ -8035,7 +8032,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>334</v>
       </c>
@@ -8052,7 +8049,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>137</v>
       </c>
@@ -8069,7 +8066,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>122</v>
       </c>
@@ -8086,7 +8083,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>448</v>
       </c>
@@ -8103,7 +8100,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>452</v>
       </c>
@@ -8120,7 +8117,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>320</v>
       </c>
@@ -8137,7 +8134,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>143</v>
       </c>
@@ -8154,7 +8151,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>146</v>
       </c>
@@ -8171,7 +8168,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>323</v>
       </c>
@@ -8191,7 +8188,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>152</v>
       </c>
@@ -8208,7 +8205,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>457</v>
       </c>
@@ -8225,7 +8222,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>326</v>
       </c>
@@ -8245,7 +8242,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>462</v>
       </c>
@@ -8262,7 +8259,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>66</v>
       </c>
@@ -8279,7 +8276,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>465</v>
       </c>
@@ -8296,7 +8293,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>158</v>
       </c>
@@ -8313,7 +8310,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>275</v>
       </c>
@@ -8330,7 +8327,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>349</v>
       </c>
@@ -8347,7 +8344,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>468</v>
       </c>
@@ -8364,7 +8361,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>328</v>
       </c>
@@ -8381,7 +8378,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>13</v>
       </c>
@@ -8401,7 +8398,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>337</v>
       </c>
@@ -8418,7 +8415,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>93</v>
       </c>
@@ -8435,7 +8432,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>472</v>
       </c>
@@ -8452,7 +8449,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>128</v>
       </c>
@@ -8469,7 +8466,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>475</v>
       </c>
@@ -8486,7 +8483,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>119</v>
       </c>
@@ -8503,7 +8500,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>476</v>
       </c>
@@ -8520,7 +8517,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>477</v>
       </c>
@@ -8537,7 +8534,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>478</v>
       </c>
@@ -8554,7 +8551,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>479</v>
       </c>
@@ -8571,7 +8568,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>315</v>
       </c>
@@ -8591,7 +8588,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>155</v>
       </c>
@@ -8616,36 +8613,35 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3036B1CA-FBEB-4E41-A2A1-61CD7E3CC4C8}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection activeCell="A109" sqref="A109"/>
-      <selection pane="topRight" activeCell="M24" sqref="M24"/>
+      <selection pane="topRight" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="3" width="42.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.81640625" customWidth="1"/>
+    <col min="3" max="3" width="42.81640625" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" customWidth="1"/>
-    <col min="12" max="12" width="33.5703125" customWidth="1"/>
-    <col min="13" max="13" width="29.28515625" customWidth="1"/>
-    <col min="14" max="14" width="40.140625" customWidth="1"/>
-    <col min="15" max="15" width="23.140625" customWidth="1"/>
-    <col min="16" max="16" width="19.85546875" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.7265625" customWidth="1"/>
+    <col min="6" max="7" width="16.7265625" customWidth="1"/>
+    <col min="8" max="8" width="20.7265625" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" customWidth="1"/>
+    <col min="11" max="11" width="20.54296875" customWidth="1"/>
+    <col min="12" max="12" width="33.54296875" customWidth="1"/>
+    <col min="13" max="13" width="29.26953125" customWidth="1"/>
+    <col min="14" max="14" width="40.1796875" customWidth="1"/>
+    <col min="15" max="15" width="23.1796875" customWidth="1"/>
+    <col min="16" max="16" width="19.81640625" customWidth="1"/>
+    <col min="17" max="17" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -8665,25 +8661,25 @@
         <v>351</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>353</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>355</v>
@@ -8696,7 +8692,7 @@
       </c>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>113</v>
       </c>
@@ -8743,7 +8739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>271</v>
       </c>
@@ -8790,7 +8786,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>311</v>
       </c>
@@ -8831,13 +8827,13 @@
         <v>115</v>
       </c>
       <c r="O4" t="s">
+        <v>367</v>
+      </c>
+      <c r="P4" t="s">
         <v>519</v>
       </c>
-      <c r="P4" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>322</v>
       </c>
@@ -8884,7 +8880,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>325</v>
       </c>
@@ -8931,7 +8927,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -8978,7 +8974,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>47</v>
       </c>
@@ -9025,7 +9021,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>50</v>
       </c>
@@ -9072,7 +9068,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>336</v>
       </c>
@@ -9119,7 +9115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>256</v>
       </c>
@@ -9166,7 +9162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>327</v>
       </c>
@@ -9213,7 +9209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>62</v>
       </c>
@@ -9260,7 +9256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>107</v>
       </c>
@@ -9310,7 +9306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>296</v>
       </c>
@@ -9357,7 +9353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>299</v>
       </c>
@@ -9404,7 +9400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>193</v>
       </c>
@@ -9455,7 +9451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>77</v>
       </c>
@@ -9502,7 +9498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>319</v>
       </c>
@@ -9549,7 +9545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>32</v>
       </c>
@@ -9593,7 +9589,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>317</v>
       </c>
@@ -9640,7 +9636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>348</v>
       </c>
@@ -9691,7 +9687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>280</v>
       </c>
@@ -9729,7 +9725,7 @@
         <v>389</v>
       </c>
       <c r="M23" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="N23" t="s">
         <v>282</v>
@@ -9741,7 +9737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>172</v>
       </c>
@@ -9791,7 +9787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>178</v>
       </c>
@@ -9841,7 +9837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>232</v>
       </c>
@@ -9892,7 +9888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>65</v>
       </c>
@@ -9930,7 +9926,7 @@
         <v>490</v>
       </c>
       <c r="N27" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="O27" t="s">
         <v>460</v>
@@ -9939,7 +9935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>166</v>
       </c>
@@ -9990,7 +9986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>139</v>
       </c>
@@ -10040,7 +10036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>53</v>
       </c>
@@ -10090,7 +10086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>259</v>
       </c>
@@ -10140,7 +10136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>169</v>
       </c>
@@ -10191,7 +10187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>244</v>
       </c>
@@ -10235,7 +10231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>253</v>
       </c>
@@ -10282,7 +10278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>214</v>
       </c>
@@ -10329,7 +10325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>229</v>
       </c>
@@ -10380,7 +10376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>148</v>
       </c>
@@ -10431,7 +10427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>286</v>
       </c>
@@ -10481,7 +10477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>95</v>
       </c>
@@ -10531,7 +10527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>71</v>
       </c>
@@ -10582,7 +10578,7 @@
       </c>
       <c r="Q40"/>
     </row>
-    <row r="41" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>175</v>
       </c>
@@ -10634,7 +10630,7 @@
       </c>
       <c r="Q41"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>250</v>
       </c>
@@ -10685,7 +10681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>283</v>
       </c>
@@ -10736,7 +10732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>83</v>
       </c>
@@ -10786,7 +10782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>104</v>
       </c>
@@ -10836,7 +10832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>157</v>
       </c>
@@ -10886,7 +10882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>11</v>
       </c>
@@ -10936,7 +10932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>187</v>
       </c>
@@ -10986,7 +10982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>235</v>
       </c>
@@ -11037,7 +11033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>184</v>
       </c>
@@ -11088,7 +11084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>92</v>
       </c>
@@ -11139,7 +11135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>7</v>
       </c>
@@ -11187,7 +11183,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="53" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>190</v>
       </c>
@@ -11239,7 +11235,7 @@
       </c>
       <c r="Q53"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
         <v>89</v>
       </c>
@@ -11290,7 +11286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>238</v>
       </c>
@@ -11341,7 +11337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>241</v>
       </c>
@@ -11392,7 +11388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:17" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>333</v>
       </c>
@@ -11412,7 +11408,7 @@
         <v>0</v>
       </c>
       <c r="G57" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H57">
         <v>1000</v>
@@ -11430,7 +11426,7 @@
         <v>433</v>
       </c>
       <c r="M57" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="N57" t="s">
         <v>335</v>
@@ -11443,7 +11439,7 @@
       </c>
       <c r="Q57"/>
     </row>
-    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>24</v>
       </c>
@@ -11490,7 +11486,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="59" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>59</v>
       </c>
@@ -11540,7 +11536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:17" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>205</v>
       </c>
@@ -11592,7 +11588,7 @@
       </c>
       <c r="Q60"/>
     </row>
-    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>211</v>
       </c>
@@ -11642,7 +11638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>217</v>
       </c>
@@ -11692,7 +11688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
         <v>220</v>
       </c>
@@ -11742,7 +11738,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>18</v>
       </c>
@@ -11789,7 +11785,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="65" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
         <v>223</v>
       </c>
@@ -11840,7 +11836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>124</v>
       </c>
@@ -11890,7 +11886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
         <v>160</v>
       </c>
@@ -11940,7 +11936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>44</v>
       </c>
@@ -11987,7 +11983,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>118</v>
       </c>
@@ -12038,7 +12034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="7" t="s">
         <v>196</v>
       </c>
@@ -12089,7 +12085,7 @@
       </c>
       <c r="Q70" s="3"/>
     </row>
-    <row r="71" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
         <v>247</v>
       </c>
@@ -12136,7 +12132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
         <v>80</v>
       </c>
@@ -12183,7 +12179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
         <v>262</v>
       </c>
@@ -12230,7 +12226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
         <v>345</v>
       </c>
@@ -12268,7 +12264,7 @@
         <v>378</v>
       </c>
       <c r="M74" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="N74" t="s">
         <v>347</v>
@@ -12280,7 +12276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
         <v>110</v>
       </c>
@@ -12327,7 +12323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
         <v>289</v>
       </c>
@@ -12378,7 +12374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
         <v>142</v>
       </c>
@@ -12429,7 +12425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>291</v>
       </c>
@@ -12476,7 +12472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
         <v>308</v>
       </c>
@@ -12523,7 +12519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
         <v>15</v>
       </c>
@@ -12567,7 +12563,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="81" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
         <v>35</v>
       </c>
@@ -12608,7 +12604,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="82" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A82" s="7" t="s">
         <v>136</v>
       </c>
@@ -12660,7 +12656,7 @@
       </c>
       <c r="Q82" s="3"/>
     </row>
-    <row r="83" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A83" s="7" t="s">
         <v>314</v>
       </c>
@@ -12712,7 +12708,7 @@
       </c>
       <c r="Q83" s="3"/>
     </row>
-    <row r="84" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
         <v>121</v>
       </c>
@@ -12763,7 +12759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>30</v>
       </c>
@@ -12807,7 +12803,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="86" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>154</v>
       </c>
@@ -12845,7 +12841,7 @@
         <v>482</v>
       </c>
       <c r="N86" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="O86" t="s">
         <v>411</v>
@@ -12854,7 +12850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
         <v>339</v>
       </c>
@@ -12892,7 +12888,7 @@
         <v>442</v>
       </c>
       <c r="N87" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="O87" t="s">
         <v>411</v>
@@ -12901,7 +12897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>151</v>
       </c>
@@ -12939,7 +12935,7 @@
         <v>442</v>
       </c>
       <c r="N88" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="O88" t="s">
         <v>411</v>
@@ -12948,7 +12944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
         <v>145</v>
       </c>
@@ -12986,7 +12982,7 @@
         <v>442</v>
       </c>
       <c r="N89" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="O89" t="s">
         <v>411</v>
@@ -12995,7 +12991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>74</v>
       </c>
@@ -13042,7 +13038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
         <v>342</v>
       </c>
@@ -13089,7 +13085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
         <v>41</v>
       </c>
@@ -13133,7 +13129,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="93" spans="1:17" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A93" s="7" t="s">
         <v>98</v>
       </c>
@@ -13184,7 +13180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
         <v>101</v>
       </c>
@@ -13234,7 +13230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="s">
         <v>274</v>
       </c>
@@ -13284,7 +13280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
         <v>38</v>
       </c>
@@ -13328,7 +13324,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="97" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
         <v>330</v>
       </c>
@@ -13375,7 +13371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A98" s="5" t="s">
         <v>226</v>
       </c>
@@ -13425,7 +13421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
         <v>68</v>
       </c>
@@ -13445,7 +13441,7 @@
         <v>0</v>
       </c>
       <c r="G99" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H99">
         <v>1</v>
@@ -13475,7 +13471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
         <v>208</v>
       </c>
@@ -13526,7 +13522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
         <v>130</v>
       </c>
@@ -13577,7 +13573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
         <v>86</v>
       </c>
@@ -13627,7 +13623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
         <v>199</v>
       </c>
@@ -13678,7 +13674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
         <v>202</v>
       </c>
@@ -13729,7 +13725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A105" s="5" t="s">
         <v>21</v>
       </c>
@@ -13776,7 +13772,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="106" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
         <v>133</v>
       </c>
@@ -13826,7 +13822,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="107" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
         <v>302</v>
       </c>
@@ -13877,7 +13873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
         <v>127</v>
       </c>
@@ -13928,7 +13924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A109" s="5" t="s">
         <v>56</v>
       </c>
@@ -13978,7 +13974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:17" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A110" s="5" t="s">
         <v>268</v>
       </c>
@@ -14029,7 +14025,7 @@
       </c>
       <c r="Q110"/>
     </row>
-    <row r="111" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A111" s="5" t="s">
         <v>163</v>
       </c>
@@ -14079,7 +14075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
         <v>305</v>
       </c>
@@ -14129,7 +14125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:17" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A113" s="5" t="s">
         <v>27</v>
       </c>
@@ -14178,7 +14174,7 @@
       <c r="P113"/>
       <c r="Q113"/>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A114" s="5" t="s">
         <v>277</v>
       </c>
@@ -14229,7 +14225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A115" s="5" t="s">
         <v>181</v>
       </c>
@@ -14280,7 +14276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A116" s="5" t="s">
         <v>294</v>
       </c>
@@ -14328,13 +14324,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q116" xr:uid="{3036B1CA-FBEB-4E41-A2A1-61CD7E3CC4C8}">
-    <filterColumn colId="11">
-      <filters>
-        <filter val="Flow"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q116">
     <sortCondition ref="B2:B116"/>
   </sortState>

</xml_diff>

<commit_message>
Units and unit groups pre-processing finalized
</commit_message>
<xml_diff>
--- a/utils/config/ReferenceLists/Units.xlsx
+++ b/utils/config/ReferenceLists/Units.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/sahil_bhandari_gov_bc_ca/Documents/teamdocs/GitHub/aqs-api/utils/config/ReferenceLists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="231" documentId="8_{7DEAA6C1-0DF4-4EB3-B17D-DC8C9B3E57AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1365963-F662-4BD8-8A00-43BC64CA836B}"/>
+  <xr:revisionPtr revIDLastSave="232" documentId="8_{7DEAA6C1-0DF4-4EB3-B17D-DC8C9B3E57AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{639F3B58-5F7C-486E-BD99-60DE16A9D642}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{BEB82E07-AA54-4E71-A23C-79CC3F3C1001}"/>
   </bookViews>
@@ -9307,7 +9307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>296</v>
       </c>
@@ -9354,7 +9354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>299</v>
       </c>
@@ -9590,7 +9590,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>317</v>
       </c>
@@ -9936,7 +9936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>166</v>
       </c>
@@ -10733,7 +10733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>83</v>
       </c>
@@ -11984,7 +11984,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>118</v>
       </c>
@@ -12426,7 +12426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>291</v>
       </c>
@@ -12473,7 +12473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
         <v>308</v>
       </c>
@@ -13325,7 +13325,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
         <v>330</v>
       </c>
@@ -14277,7 +14277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" s="5" t="s">
         <v>294</v>
       </c>
@@ -14328,7 +14328,7 @@
   <autoFilter ref="A1:Q116" xr:uid="{3036B1CA-FBEB-4E41-A2A1-61CD7E3CC4C8}">
     <filterColumn colId="11">
       <filters>
-        <filter val="Count"/>
+        <filter val="Length"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>